<commit_message>
Compare expression patterns between esfenvalerate and rag1
</commit_message>
<xml_diff>
--- a/foldchanges.xlsx
+++ b/foldchanges.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Thiamethoxam" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="156">
   <si>
     <t>sba_whole_aphid_contig_4531:PREDICTED:probable_cytochrome_P450_6a13-like[Acyrthosiphon_pisum]</t>
   </si>
@@ -1095,6 +1095,9 @@
   </si>
   <si>
     <t>sba_whole_aphid_contig_4913:PREDICTED:similar_to_fumarylacetoacetate_hydrolase[Tribolium_castaneum]_&gt;gi|270009995|gb|EFA06443.1|_hypothetical_protein_TcasGA2_TC009325[Tribolium_castaneum]</t>
+  </si>
+  <si>
+    <t>transcript</t>
   </si>
 </sst>
 </file>
@@ -1222,8 +1225,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1275,15 +1280,17 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1613,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1624,7 +1631,7 @@
     <col min="1" max="1" width="138" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1">
+    <row r="1" spans="1:4" ht="16" thickBot="1">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1634,8 +1641,11 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1">
+      <c r="D1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1645,8 +1655,12 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1">
+      <c r="D2" t="str">
+        <f>LEFT(A2, SEARCH(":",A2))</f>
+        <v>sba_whole_aphid_contig_4531:</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1657,8 +1671,12 @@
         <f>C2</f>
         <v>p450</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D50" si="0">LEFT(A3, SEARCH(":",A3))</f>
+        <v>sba_whole_aphid_contig_6666:</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1669,8 +1687,12 @@
         <f>C3</f>
         <v>p450</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_1380:</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1680,8 +1702,12 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_7070:</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1691,8 +1717,12 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13671:</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1702,8 +1732,12 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="16" thickBot="1">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_3488:</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -1713,8 +1747,12 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="16" thickBot="1">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13246:</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -1724,8 +1762,12 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_12455:</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1735,8 +1777,12 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" thickBot="1">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_2990:</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -1746,8 +1792,12 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_3277:</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -1757,8 +1807,12 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="16" thickBot="1">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_14746:</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -1768,8 +1822,12 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_11825:</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1779,8 +1837,12 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="16" thickBot="1">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_436:</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -1790,8 +1852,12 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_1839:</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -1801,8 +1867,12 @@
       <c r="C16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="16" thickBot="1">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_12749:</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -1812,8 +1882,12 @@
       <c r="C17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_5657:</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -1823,8 +1897,12 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="16" thickBot="1">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_4993:</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" thickBot="1">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1834,8 +1912,12 @@
       <c r="C19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="16" thickBot="1">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_2821:</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -1845,8 +1927,12 @@
       <c r="C20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="16" thickBot="1">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_10996:</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" thickBot="1">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1856,8 +1942,12 @@
       <c r="C21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="16" thickBot="1">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_15004:</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" thickBot="1">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
@@ -1867,8 +1957,12 @@
       <c r="C22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="25" thickBot="1">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_11126:</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="25" thickBot="1">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1878,8 +1972,12 @@
       <c r="C23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="25" thickBot="1">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_11204:</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="25" thickBot="1">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -1889,8 +1987,12 @@
       <c r="C24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="16" thickBot="1">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_5532:</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1900,8 +2002,12 @@
       <c r="C25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="16" thickBot="1">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_4186:</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" thickBot="1">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
@@ -1911,8 +2017,12 @@
       <c r="C26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="16" thickBot="1">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13304:</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
@@ -1922,8 +2032,12 @@
       <c r="C27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="16" thickBot="1">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_10390:</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" thickBot="1">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
@@ -1933,8 +2047,12 @@
       <c r="C28" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="16" thickBot="1">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_7015:</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" thickBot="1">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
@@ -1944,8 +2062,12 @@
       <c r="C29" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="16" thickBot="1">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_11390:</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" thickBot="1">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
@@ -1955,8 +2077,12 @@
       <c r="C30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="16" thickBot="1">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13246:</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" thickBot="1">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -1966,8 +2092,12 @@
       <c r="C31" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="25" thickBot="1">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_9541:</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="25" thickBot="1">
       <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
@@ -1977,8 +2107,12 @@
       <c r="C32" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="16" thickBot="1">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_2632:</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" thickBot="1">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
@@ -1988,8 +2122,12 @@
       <c r="C33" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="25" thickBot="1">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_8446:</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="25" thickBot="1">
       <c r="A34" s="3" t="s">
         <v>37</v>
       </c>
@@ -1999,8 +2137,12 @@
       <c r="C34" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="16" thickBot="1">
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_8362:</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" thickBot="1">
       <c r="A35" s="3" t="s">
         <v>38</v>
       </c>
@@ -2010,8 +2152,12 @@
       <c r="C35" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="16" thickBot="1">
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13827:</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16" thickBot="1">
       <c r="A36" s="3" t="s">
         <v>39</v>
       </c>
@@ -2021,8 +2167,12 @@
       <c r="C36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="37" thickBot="1">
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_12918:</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="37" thickBot="1">
       <c r="A37" s="3" t="s">
         <v>40</v>
       </c>
@@ -2032,8 +2182,12 @@
       <c r="C37" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="16" thickBot="1">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_6657:</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>41</v>
       </c>
@@ -2043,8 +2197,12 @@
       <c r="C38" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="16" thickBot="1">
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_9343:</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16" thickBot="1">
       <c r="A39" s="3" t="s">
         <v>42</v>
       </c>
@@ -2054,8 +2212,12 @@
       <c r="C39" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="16" thickBot="1">
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_1802:</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16" thickBot="1">
       <c r="A40" s="3" t="s">
         <v>43</v>
       </c>
@@ -2065,8 +2227,12 @@
       <c r="C40" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="16" thickBot="1">
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_6912:</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>44</v>
       </c>
@@ -2076,8 +2242,12 @@
       <c r="C41" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" thickBot="1">
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_15151:</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16" thickBot="1">
       <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
@@ -2087,8 +2257,12 @@
       <c r="C42" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="16" thickBot="1">
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_440:</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16" thickBot="1">
       <c r="A43" s="3" t="s">
         <v>46</v>
       </c>
@@ -2098,8 +2272,12 @@
       <c r="C43" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="37" thickBot="1">
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_10231:</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="37" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>47</v>
       </c>
@@ -2109,8 +2287,12 @@
       <c r="C44" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="16" thickBot="1">
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_9011:</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="16" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>48</v>
       </c>
@@ -2120,8 +2302,12 @@
       <c r="C45" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" thickBot="1">
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_10612:</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="16" thickBot="1">
       <c r="A46" s="5" t="s">
         <v>50</v>
       </c>
@@ -2131,8 +2317,12 @@
       <c r="C46" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="16" thickBot="1">
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_10858:</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16" thickBot="1">
       <c r="A47" s="7" t="s">
         <v>51</v>
       </c>
@@ -2142,8 +2332,12 @@
       <c r="C47" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="16" thickBot="1">
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_7898:</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="16" thickBot="1">
       <c r="A48" s="7" t="s">
         <v>52</v>
       </c>
@@ -2153,8 +2347,12 @@
       <c r="C48" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="16" thickBot="1">
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_9997:</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="16" thickBot="1">
       <c r="A49" s="7" t="s">
         <v>53</v>
       </c>
@@ -2164,8 +2362,12 @@
       <c r="C49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="16" thickBot="1">
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_7780:</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="16" thickBot="1">
       <c r="A50" s="7" t="s">
         <v>54</v>
       </c>
@@ -2174,6 +2376,10 @@
       </c>
       <c r="C50" t="s">
         <v>49</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_5586:</v>
       </c>
     </row>
   </sheetData>
@@ -2189,10 +2395,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106:C117"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2200,7 +2406,7 @@
     <col min="1" max="1" width="141.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1">
+    <row r="1" spans="1:4" ht="16" thickBot="1">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2210,8 +2416,11 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1">
+      <c r="D1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2221,8 +2430,12 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1">
+      <c r="D2" t="str">
+        <f>LEFT(A2, SEARCH(":",A2))</f>
+        <v>sba_whole_aphid_contig_1380:</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>55</v>
       </c>
@@ -2233,8 +2446,12 @@
         <f>C2</f>
         <v>p450</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="0">LEFT(A3, SEARCH(":",A3))</f>
+        <v>sba_whole_aphid_contig_14715:</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>56</v>
       </c>
@@ -2242,11 +2459,15 @@
         <v>-0.51146185942919997</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C24" si="0">C3</f>
+        <f t="shared" ref="C4:C24" si="1">C3</f>
         <v>p450</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_1639:</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>57</v>
       </c>
@@ -2254,11 +2475,15 @@
         <v>-0.65883005542850004</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_8206:</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>58</v>
       </c>
@@ -2266,11 +2491,15 @@
         <v>-0.76405761334139999</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_15277:</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>59</v>
       </c>
@@ -2278,11 +2507,15 @@
         <v>-0.82653333535745999</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="16" thickBot="1">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_975:</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -2290,11 +2523,15 @@
         <v>0.52637066721000003</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="16" thickBot="1">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_6666:</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>60</v>
       </c>
@@ -2302,11 +2539,15 @@
         <v>0.52684468225000003</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_10452:</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>61</v>
       </c>
@@ -2314,11 +2555,15 @@
         <v>0.70190465797000001</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" thickBot="1">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_14313:</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>62</v>
       </c>
@@ -2326,11 +2571,15 @@
         <v>0.75366159510999997</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="25" thickBot="1">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_14438:</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="25" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>63</v>
       </c>
@@ -2338,11 +2587,15 @@
         <v>0.76213914532000004</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="16" thickBot="1">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_5703:</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>64</v>
       </c>
@@ -2350,11 +2603,15 @@
         <v>0.82395739482999997</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_8279:</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>65</v>
       </c>
@@ -2362,11 +2619,15 @@
         <v>0.82872994692000002</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="16" thickBot="1">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_9739:</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>66</v>
       </c>
@@ -2374,11 +2635,15 @@
         <v>0.85300261272</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_10092:</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>67</v>
       </c>
@@ -2386,11 +2651,15 @@
         <v>0.90152345024000002</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="16" thickBot="1">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_12532:</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" thickBot="1">
       <c r="A17" s="9" t="s">
         <v>68</v>
       </c>
@@ -2398,11 +2667,15 @@
         <v>0.94358045524</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_3547:</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>69</v>
       </c>
@@ -2410,11 +2683,15 @@
         <v>0.95222011417999997</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="16" thickBot="1">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_14460:</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" thickBot="1">
       <c r="A19" s="3" t="s">
         <v>70</v>
       </c>
@@ -2422,11 +2699,15 @@
         <v>0.95369309150000003</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="16" thickBot="1">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_15283:</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>71</v>
       </c>
@@ -2434,11 +2715,15 @@
         <v>1.01153263809</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="16" thickBot="1">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_8141:</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>72</v>
       </c>
@@ -2446,11 +2731,15 @@
         <v>1.0927538049400001</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="16" thickBot="1">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_7883:</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>73</v>
       </c>
@@ -2458,11 +2747,15 @@
         <v>1.1706471836400001</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="16" thickBot="1">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_8318:</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" thickBot="1">
       <c r="A23" s="3" t="s">
         <v>74</v>
       </c>
@@ -2470,11 +2763,15 @@
         <v>1.23533857653</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="16" thickBot="1">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_12169:</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" thickBot="1">
       <c r="A24" s="3" t="s">
         <v>0</v>
       </c>
@@ -2482,11 +2779,15 @@
         <v>1.35353540363</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>p450</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="16" thickBot="1">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_4531:</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" thickBot="1">
       <c r="A25" s="10" t="s">
         <v>75</v>
       </c>
@@ -2496,8 +2797,12 @@
       <c r="C25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="16" thickBot="1">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_7070:</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -2507,8 +2812,12 @@
       <c r="C26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="16" thickBot="1">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_4921:</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>77</v>
       </c>
@@ -2518,8 +2827,12 @@
       <c r="C27" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="16" thickBot="1">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_6834:</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" thickBot="1">
       <c r="A28" s="10" t="s">
         <v>78</v>
       </c>
@@ -2529,8 +2842,12 @@
       <c r="C28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="16" thickBot="1">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_7418:</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" thickBot="1">
       <c r="A29" s="12" t="s">
         <v>79</v>
       </c>
@@ -2540,8 +2857,12 @@
       <c r="C29" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="16" thickBot="1">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_3488:</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" thickBot="1">
       <c r="A30" s="12" t="s">
         <v>80</v>
       </c>
@@ -2551,8 +2872,12 @@
       <c r="C30" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="16" thickBot="1">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_8125:</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" thickBot="1">
       <c r="A31" s="12" t="s">
         <v>81</v>
       </c>
@@ -2562,8 +2887,12 @@
       <c r="C31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="16" thickBot="1">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13246:</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16" thickBot="1">
       <c r="A32" s="12" t="s">
         <v>82</v>
       </c>
@@ -2573,8 +2902,12 @@
       <c r="C32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="16" thickBot="1">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_1729:</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" thickBot="1">
       <c r="A33" s="12" t="s">
         <v>83</v>
       </c>
@@ -2584,8 +2917,12 @@
       <c r="C33" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="16" thickBot="1">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_4151:</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" thickBot="1">
       <c r="A34" s="12" t="s">
         <v>84</v>
       </c>
@@ -2595,8 +2932,12 @@
       <c r="C34" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="16" thickBot="1">
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_12455:</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" thickBot="1">
       <c r="A35" s="12" t="s">
         <v>85</v>
       </c>
@@ -2606,8 +2947,12 @@
       <c r="C35" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="16" thickBot="1">
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13671:</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16" thickBot="1">
       <c r="A36" s="12" t="s">
         <v>86</v>
       </c>
@@ -2617,8 +2962,12 @@
       <c r="C36" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="16" thickBot="1">
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_12135:</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" thickBot="1">
       <c r="A37" s="12" t="s">
         <v>87</v>
       </c>
@@ -2628,8 +2977,12 @@
       <c r="C37" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="16" thickBot="1">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_12749:</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16" thickBot="1">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -2639,8 +2992,12 @@
       <c r="C38" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="25" thickBot="1">
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_14569:</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="25" thickBot="1">
       <c r="A39" s="12" t="s">
         <v>89</v>
       </c>
@@ -2650,8 +3007,12 @@
       <c r="C39" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="16" thickBot="1">
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13133:</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16" thickBot="1">
       <c r="A40" s="12" t="s">
         <v>90</v>
       </c>
@@ -2661,8 +3022,12 @@
       <c r="C40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="16" thickBot="1">
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_6945:</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16" thickBot="1">
       <c r="A41" s="12" t="s">
         <v>91</v>
       </c>
@@ -2672,8 +3037,12 @@
       <c r="C41" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" thickBot="1">
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_14746:</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16" thickBot="1">
       <c r="A42" s="12" t="s">
         <v>92</v>
       </c>
@@ -2683,8 +3052,12 @@
       <c r="C42" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="16" thickBot="1">
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_2990:</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16" thickBot="1">
       <c r="A43" s="12" t="s">
         <v>93</v>
       </c>
@@ -2694,8 +3067,12 @@
       <c r="C43" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="16" thickBot="1">
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_3277:</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>94</v>
       </c>
@@ -2705,8 +3082,12 @@
       <c r="C44" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="16" thickBot="1">
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_436:</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="16" thickBot="1">
       <c r="A45" s="12" t="s">
         <v>95</v>
       </c>
@@ -2716,8 +3097,12 @@
       <c r="C45" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" thickBot="1">
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_5657:</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="16" thickBot="1">
       <c r="A46" s="12" t="s">
         <v>96</v>
       </c>
@@ -2727,8 +3112,12 @@
       <c r="C46" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="16" thickBot="1">
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_11825:</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16" thickBot="1">
       <c r="A47" s="12" t="s">
         <v>97</v>
       </c>
@@ -2738,8 +3127,12 @@
       <c r="C47" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="16" thickBot="1">
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_2908:</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="16" thickBot="1">
       <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
@@ -2749,8 +3142,12 @@
       <c r="C48" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="25" thickBot="1">
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_1847:</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="25" thickBot="1">
       <c r="A49" s="3" t="s">
         <v>99</v>
       </c>
@@ -2760,8 +3157,12 @@
       <c r="C49" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="16" thickBot="1">
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_15423:</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="16" thickBot="1">
       <c r="A50" s="3" t="s">
         <v>22</v>
       </c>
@@ -2771,8 +3172,12 @@
       <c r="C50" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="16" thickBot="1">
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_4993:</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="16" thickBot="1">
       <c r="A51" s="3" t="s">
         <v>26</v>
       </c>
@@ -2782,8 +3187,12 @@
       <c r="C51" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="16" thickBot="1">
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_11126:</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="16" thickBot="1">
       <c r="A52" s="3" t="s">
         <v>24</v>
       </c>
@@ -2793,8 +3202,12 @@
       <c r="C52" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="16" thickBot="1">
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_10996:</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="16" thickBot="1">
       <c r="A53" s="3" t="s">
         <v>100</v>
       </c>
@@ -2804,8 +3217,12 @@
       <c r="C53" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="16" thickBot="1">
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_11692:</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="16" thickBot="1">
       <c r="A54" s="3" t="s">
         <v>101</v>
       </c>
@@ -2815,8 +3232,12 @@
       <c r="C54" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="16" thickBot="1">
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_14528:</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="16" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>25</v>
       </c>
@@ -2826,8 +3247,12 @@
       <c r="C55" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="16" thickBot="1">
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_15004:</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="16" thickBot="1">
       <c r="A56" s="3" t="s">
         <v>102</v>
       </c>
@@ -2837,8 +3262,12 @@
       <c r="C56" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="16" thickBot="1">
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_1859:</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="16" thickBot="1">
       <c r="A57" s="3" t="s">
         <v>23</v>
       </c>
@@ -2848,8 +3277,12 @@
       <c r="C57" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="16" thickBot="1">
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_2821:</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="16" thickBot="1">
       <c r="A58" s="3" t="s">
         <v>103</v>
       </c>
@@ -2859,8 +3292,12 @@
       <c r="C58" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="16" thickBot="1">
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_11436:</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="16" thickBot="1">
       <c r="A59" s="3" t="s">
         <v>104</v>
       </c>
@@ -2870,8 +3307,12 @@
       <c r="C59" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="16" thickBot="1">
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13089:</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="16" thickBot="1">
       <c r="A60" s="3" t="s">
         <v>105</v>
       </c>
@@ -2881,8 +3322,12 @@
       <c r="C60" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="16" thickBot="1">
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_4740:</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="16" thickBot="1">
       <c r="A61" s="3" t="s">
         <v>106</v>
       </c>
@@ -2892,8 +3337,12 @@
       <c r="C61" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="16" thickBot="1">
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_811:</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="16" thickBot="1">
       <c r="A62" s="3" t="s">
         <v>107</v>
       </c>
@@ -2903,8 +3352,12 @@
       <c r="C62" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="25" thickBot="1">
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_14216:</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="25" thickBot="1">
       <c r="A63" s="3" t="s">
         <v>28</v>
       </c>
@@ -2914,8 +3367,12 @@
       <c r="C63" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="16" thickBot="1">
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_5532:</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="16" thickBot="1">
       <c r="A64" s="3" t="s">
         <v>108</v>
       </c>
@@ -2925,8 +3382,12 @@
       <c r="C64" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="25" thickBot="1">
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_2379:</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="25" thickBot="1">
       <c r="A65" s="3" t="s">
         <v>27</v>
       </c>
@@ -2936,8 +3397,12 @@
       <c r="C65" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" thickBot="1">
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_11204:</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="16" thickBot="1">
       <c r="A66" s="10" t="s">
         <v>109</v>
       </c>
@@ -2947,8 +3412,12 @@
       <c r="C66" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" thickBot="1">
+      <c r="D66" t="str">
+        <f t="shared" si="0"/>
+        <v>sba_whole_aphid_contig_13304:</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="16" thickBot="1">
       <c r="A67" s="12" t="s">
         <v>110</v>
       </c>
@@ -2958,8 +3427,12 @@
       <c r="C67" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="16" thickBot="1">
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D117" si="2">LEFT(A67, SEARCH(":",A67))</f>
+        <v>sba_whole_aphid_contig_12960:</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="16" thickBot="1">
       <c r="A68" s="12" t="s">
         <v>111</v>
       </c>
@@ -2969,8 +3442,12 @@
       <c r="C68" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="16" thickBot="1">
+      <c r="D68" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_657:</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="16" thickBot="1">
       <c r="A69" s="12" t="s">
         <v>112</v>
       </c>
@@ -2980,8 +3457,12 @@
       <c r="C69" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="16" thickBot="1">
+      <c r="D69" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_10390:</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="16" thickBot="1">
       <c r="A70" s="12" t="s">
         <v>113</v>
       </c>
@@ -2991,8 +3472,12 @@
       <c r="C70" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="16" thickBot="1">
+      <c r="D70" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_13827:</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="16" thickBot="1">
       <c r="A71" s="12" t="s">
         <v>114</v>
       </c>
@@ -3002,8 +3487,12 @@
       <c r="C71" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="16" thickBot="1">
+      <c r="D71" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_7766:</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="16" thickBot="1">
       <c r="A72" s="12" t="s">
         <v>115</v>
       </c>
@@ -3013,8 +3502,12 @@
       <c r="C72" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="16" thickBot="1">
+      <c r="D72" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_11390:</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="16" thickBot="1">
       <c r="A73" s="12" t="s">
         <v>116</v>
       </c>
@@ -3024,8 +3517,12 @@
       <c r="C73" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="16" thickBot="1">
+      <c r="D73" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_6912:</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="16" thickBot="1">
       <c r="A74" s="12" t="s">
         <v>117</v>
       </c>
@@ -3035,8 +3532,12 @@
       <c r="C74" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="16" thickBot="1">
+      <c r="D74" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_9541:</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="16" thickBot="1">
       <c r="A75" s="12" t="s">
         <v>118</v>
       </c>
@@ -3046,8 +3547,12 @@
       <c r="C75" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" thickBot="1">
+      <c r="D75" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_11768:</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="16" thickBot="1">
       <c r="A76" s="12" t="s">
         <v>81</v>
       </c>
@@ -3057,8 +3562,12 @@
       <c r="C76" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" thickBot="1">
+      <c r="D76" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_13246:</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="16" thickBot="1">
       <c r="A77" s="12" t="s">
         <v>119</v>
       </c>
@@ -3068,8 +3577,12 @@
       <c r="C77" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="16" thickBot="1">
+      <c r="D77" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_14511:</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="16" thickBot="1">
       <c r="A78" s="12" t="s">
         <v>120</v>
       </c>
@@ -3079,8 +3592,12 @@
       <c r="C78" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" thickBot="1">
+      <c r="D78" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_13145:</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="16" thickBot="1">
       <c r="A79" s="12" t="s">
         <v>121</v>
       </c>
@@ -3090,8 +3607,12 @@
       <c r="C79" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="25" thickBot="1">
+      <c r="D79" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_7015:</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="25" thickBot="1">
       <c r="A80" s="12" t="s">
         <v>122</v>
       </c>
@@ -3101,8 +3622,12 @@
       <c r="C80" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" ht="16" thickBot="1">
+      <c r="D80" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_8362:</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="16" thickBot="1">
       <c r="A81" s="12" t="s">
         <v>123</v>
       </c>
@@ -3112,8 +3637,12 @@
       <c r="C81" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="16" thickBot="1">
+      <c r="D81" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_2632:</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="16" thickBot="1">
       <c r="A82" s="12" t="s">
         <v>124</v>
       </c>
@@ -3123,8 +3652,12 @@
       <c r="C82" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="16" thickBot="1">
+      <c r="D82" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_2224:</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="16" thickBot="1">
       <c r="A83" s="12" t="s">
         <v>125</v>
       </c>
@@ -3134,8 +3667,12 @@
       <c r="C83" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="25" thickBot="1">
+      <c r="D83" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_2322:</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="25" thickBot="1">
       <c r="A84" s="12" t="s">
         <v>126</v>
       </c>
@@ -3145,8 +3682,12 @@
       <c r="C84" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" ht="37" thickBot="1">
+      <c r="D84" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_9415:</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="37" thickBot="1">
       <c r="A85" s="12" t="s">
         <v>127</v>
       </c>
@@ -3156,8 +3697,12 @@
       <c r="C85" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="16" thickBot="1">
+      <c r="D85" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_6657:</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="16" thickBot="1">
       <c r="A86" s="12" t="s">
         <v>128</v>
       </c>
@@ -3167,8 +3712,12 @@
       <c r="C86" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="16" thickBot="1">
+      <c r="D86" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_15154:</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="16" thickBot="1">
       <c r="A87" s="12" t="s">
         <v>129</v>
       </c>
@@ -3178,8 +3727,12 @@
       <c r="C87" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="16" thickBot="1">
+      <c r="D87" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_12918:</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="16" thickBot="1">
       <c r="A88" s="12" t="s">
         <v>130</v>
       </c>
@@ -3189,8 +3742,12 @@
       <c r="C88" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="16" thickBot="1">
+      <c r="D88" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_14388:</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="16" thickBot="1">
       <c r="A89" s="12" t="s">
         <v>131</v>
       </c>
@@ -3200,8 +3757,12 @@
       <c r="C89" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="16" thickBot="1">
+      <c r="D89" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_14089:</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="16" thickBot="1">
       <c r="A90" s="12" t="s">
         <v>132</v>
       </c>
@@ -3211,8 +3772,12 @@
       <c r="C90" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="25" thickBot="1">
+      <c r="D90" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_14265:</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="25" thickBot="1">
       <c r="A91" s="12" t="s">
         <v>133</v>
       </c>
@@ -3222,8 +3787,12 @@
       <c r="C91" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="16" thickBot="1">
+      <c r="D91" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_14283:</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="16" thickBot="1">
       <c r="A92" s="12" t="s">
         <v>134</v>
       </c>
@@ -3233,8 +3802,12 @@
       <c r="C92" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="16" thickBot="1">
+      <c r="D92" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_8377:</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="16" thickBot="1">
       <c r="A93" s="12" t="s">
         <v>135</v>
       </c>
@@ -3244,8 +3817,12 @@
       <c r="C93" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="16" thickBot="1">
+      <c r="D93" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_15151:</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="16" thickBot="1">
       <c r="A94" s="12" t="s">
         <v>136</v>
       </c>
@@ -3255,8 +3832,12 @@
       <c r="C94" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" ht="16" thickBot="1">
+      <c r="D94" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_1802:</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="16" thickBot="1">
       <c r="A95" s="12" t="s">
         <v>137</v>
       </c>
@@ -3266,8 +3847,12 @@
       <c r="C95" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="16" thickBot="1">
+      <c r="D95" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_8446:</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="16" thickBot="1">
       <c r="A96" s="12" t="s">
         <v>138</v>
       </c>
@@ -3277,8 +3862,12 @@
       <c r="C96" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="25" thickBot="1">
+      <c r="D96" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_1957:</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="25" thickBot="1">
       <c r="A97" s="12" t="s">
         <v>139</v>
       </c>
@@ -3288,8 +3877,12 @@
       <c r="C97" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="16" thickBot="1">
+      <c r="D97" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_14778:</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="16" thickBot="1">
       <c r="A98" s="12" t="s">
         <v>140</v>
       </c>
@@ -3299,8 +3892,12 @@
       <c r="C98" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" ht="16" thickBot="1">
+      <c r="D98" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_10612:</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="16" thickBot="1">
       <c r="A99" s="12" t="s">
         <v>141</v>
       </c>
@@ -3310,8 +3907,12 @@
       <c r="C99" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="16" thickBot="1">
+      <c r="D99" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_9343:</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="16" thickBot="1">
       <c r="A100" s="12" t="s">
         <v>142</v>
       </c>
@@ -3321,8 +3922,12 @@
       <c r="C100" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="16" thickBot="1">
+      <c r="D100" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_10231:</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="16" thickBot="1">
       <c r="A101" s="12" t="s">
         <v>143</v>
       </c>
@@ -3332,8 +3937,12 @@
       <c r="C101" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" ht="16" thickBot="1">
+      <c r="D101" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_440:</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="16" thickBot="1">
       <c r="A102" s="12" t="s">
         <v>144</v>
       </c>
@@ -3343,8 +3952,12 @@
       <c r="C102" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="16" thickBot="1">
+      <c r="D102" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_3208:</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="16" thickBot="1">
       <c r="A103" s="12" t="s">
         <v>145</v>
       </c>
@@ -3354,8 +3967,12 @@
       <c r="C103" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" ht="37" thickBot="1">
+      <c r="D103" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_11048:</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="37" thickBot="1">
       <c r="A104" s="12" t="s">
         <v>146</v>
       </c>
@@ -3365,8 +3982,12 @@
       <c r="C104" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" ht="25" thickBot="1">
+      <c r="D104" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_9011:</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="25" thickBot="1">
       <c r="A105" s="12" t="s">
         <v>147</v>
       </c>
@@ -3376,8 +3997,12 @@
       <c r="C105" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" ht="25" thickBot="1">
+      <c r="D105" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_3998:</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="25" thickBot="1">
       <c r="A106" s="12" t="s">
         <v>148</v>
       </c>
@@ -3387,8 +4012,12 @@
       <c r="C106" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" ht="25" thickBot="1">
+      <c r="D106" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_3358:</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="25" thickBot="1">
       <c r="A107" s="1" t="s">
         <v>149</v>
       </c>
@@ -3398,8 +4027,12 @@
       <c r="C107" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" ht="16" thickBot="1">
+      <c r="D107" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_7767:</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="16" thickBot="1">
       <c r="A108" s="3" t="s">
         <v>51</v>
       </c>
@@ -3409,8 +4042,12 @@
       <c r="C108" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" ht="16" thickBot="1">
+      <c r="D108" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_7898:</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="16" thickBot="1">
       <c r="A109" s="3" t="s">
         <v>150</v>
       </c>
@@ -3420,8 +4057,12 @@
       <c r="C109" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" ht="16" thickBot="1">
+      <c r="D109" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_4399:</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="16" thickBot="1">
       <c r="A110" s="3" t="s">
         <v>50</v>
       </c>
@@ -3431,8 +4072,12 @@
       <c r="C110" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="16" thickBot="1">
+      <c r="D110" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_10858:</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="16" thickBot="1">
       <c r="A111" s="3" t="s">
         <v>151</v>
       </c>
@@ -3442,8 +4087,12 @@
       <c r="C111" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="16" thickBot="1">
+      <c r="D111" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_9129:</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="16" thickBot="1">
       <c r="A112" s="3" t="s">
         <v>52</v>
       </c>
@@ -3453,8 +4102,12 @@
       <c r="C112" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" ht="16" thickBot="1">
+      <c r="D112" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_9997:</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="16" thickBot="1">
       <c r="A113" s="3" t="s">
         <v>152</v>
       </c>
@@ -3464,8 +4117,12 @@
       <c r="C113" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="16" thickBot="1">
+      <c r="D113" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_13111:</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="16" thickBot="1">
       <c r="A114" s="3" t="s">
         <v>53</v>
       </c>
@@ -3475,8 +4132,12 @@
       <c r="C114" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" ht="16" thickBot="1">
+      <c r="D114" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_7780:</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="16" thickBot="1">
       <c r="A115" s="3" t="s">
         <v>153</v>
       </c>
@@ -3486,8 +4147,12 @@
       <c r="C115" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" ht="25" thickBot="1">
+      <c r="D115" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_1979:</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="25" thickBot="1">
       <c r="A116" s="3" t="s">
         <v>154</v>
       </c>
@@ -3497,8 +4162,12 @@
       <c r="C116" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" ht="16" thickBot="1">
+      <c r="D116" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_4913:</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="16" thickBot="1">
       <c r="A117" s="3" t="s">
         <v>54</v>
       </c>
@@ -3508,9 +4177,14 @@
       <c r="C117" t="s">
         <v>49</v>
       </c>
+      <c r="D117" t="str">
+        <f t="shared" si="2"/>
+        <v>sba_whole_aphid_contig_5586:</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>